<commit_message>
loading in newest US data
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BPSfDSPC/BAU Perc Subsidy for Distributed Solar PV Capacity.xlsx
+++ b/InputData/bldgs/BPSfDSPC/BAU Perc Subsidy for Distributed Solar PV Capacity.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\bldgs\BPSfDSPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\bldgs\BPSfDSPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6790632B-7370-4F44-8D4A-453872B4A6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B358AC65-4386-4D6B-A447-C59C227A0A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="24240" windowHeight="14730" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="7" r:id="rId1"/>
-    <sheet name="BPSfDSPC" sheetId="8" r:id="rId2"/>
+    <sheet name="BPSfDSPV" sheetId="8" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -111,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -121,6 +121,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -140,9 +141,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -180,9 +181,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,9 +216,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,9 +268,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,10 +461,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -448,7 +482,7 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -468,13 +502,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet2">
+  <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,94 +616,94 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="N2" s="5">
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="N2" s="6">
         <v>0.26</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="6">
         <v>0.22</v>
       </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>0</v>
-      </c>
-      <c r="R2" s="5">
-        <v>0</v>
-      </c>
-      <c r="S2" s="5">
-        <v>0</v>
-      </c>
-      <c r="T2" s="5">
-        <v>0</v>
-      </c>
-      <c r="U2" s="5">
-        <v>0</v>
-      </c>
-      <c r="V2" s="5">
-        <v>0</v>
-      </c>
-      <c r="W2" s="5">
-        <v>0</v>
-      </c>
-      <c r="X2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="5">
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0</v>
+      </c>
+      <c r="U2" s="6">
+        <v>0</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0</v>
+      </c>
+      <c r="X2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="6">
         <v>0</v>
       </c>
     </row>
@@ -677,94 +711,94 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="N3" s="5">
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="N3" s="6">
         <v>0.26</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="6">
         <v>0.22</v>
       </c>
-      <c r="P3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
-        <v>0</v>
-      </c>
-      <c r="S3" s="5">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
-        <v>0</v>
-      </c>
-      <c r="W3" s="5">
-        <v>0</v>
-      </c>
-      <c r="X3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="5">
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0</v>
+      </c>
+      <c r="T3" s="6">
+        <v>0</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0</v>
+      </c>
+      <c r="V3" s="6">
+        <v>0</v>
+      </c>
+      <c r="W3" s="6">
+        <v>0</v>
+      </c>
+      <c r="X3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="6">
         <v>0</v>
       </c>
     </row>
@@ -772,94 +806,94 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-      <c r="M4" s="5">
-        <v>0</v>
-      </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="O4" s="5">
-        <v>0</v>
-      </c>
-      <c r="P4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>0</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0</v>
-      </c>
-      <c r="S4" s="5">
-        <v>0</v>
-      </c>
-      <c r="T4" s="5">
-        <v>0</v>
-      </c>
-      <c r="U4" s="5">
-        <v>0</v>
-      </c>
-      <c r="V4" s="5">
-        <v>0</v>
-      </c>
-      <c r="W4" s="5">
-        <v>0</v>
-      </c>
-      <c r="X4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="5">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="5">
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6">
+        <v>0</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>